<commit_message>
actualización de resultados con ajustes de pylint
</commit_message>
<xml_diff>
--- a/A01797560_A5.2/results/P1 RESULTS.xlsx
+++ b/A01797560_A5.2/results/P1 RESULTS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vjuarezc\PycharmProjects\Pruebas-y-Calidad\A01797560_A5.2\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C49B5A2-51E3-4270-A15E-C7556739CC7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E8A3F2-3FD9-4A04-9025-55B5CD157349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,8 @@
     <sheet name="TC1" sheetId="1" r:id="rId1"/>
     <sheet name="TC2" sheetId="2" r:id="rId2"/>
     <sheet name="TC3" sheetId="3" r:id="rId3"/>
-    <sheet name="flake8" sheetId="7" r:id="rId4"/>
+    <sheet name="pylint" sheetId="8" r:id="rId4"/>
+    <sheet name="flake8" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -325,10 +326,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7A7FBA0-4090-61AD-60F9-AED31E13A4B7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AAF6D42B-9424-187C-698B-6D957D765983}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -374,10 +375,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCA23C3C-DDB0-30B2-EFFE-79D0E53768BF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7687FAD-9A73-2D93-2669-64B43038680E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -423,10 +424,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5177038B-941A-CC3B-9A6D-F4E25A244A0C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{748D64AF-D19E-6F47-241E-020464FEB3D6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -475,7 +476,56 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56EE86E9-BA63-D369-DE4D-460D38F3CC2B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D173C47-BDC4-CDD2-21A3-94D33A3F3758}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="18285714" cy="10285714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>607314</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>157464</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9FDDF7E2-66FC-F53C-0FB4-6BF04627918C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -764,7 +814,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.81640625" defaultRowHeight="14.5"/>
   <cols>
@@ -796,7 +846,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A12628"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0"/>
+    <sheetView topLeftCell="A25" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
@@ -813,6 +863,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F48889EA-983D-4C03-B74D-B1E7B56915F7}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A34" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>